<commit_message>
GB Red model added
</commit_message>
<xml_diff>
--- a/OATS-testcases/case24_ieee_rts.xlsx
+++ b/OATS-testcases/case24_ieee_rts.xlsx
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2218,7 +2218,7 @@
   <dimension ref="A1:AL1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3127,7 +3127,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="2:3 J24"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3164,7 +3164,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="2:3 B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3551,7 +3551,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="2:3 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="2:215 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4972,7 +4972,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5332,10 +5332,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="2:3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A182" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A215" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5386,6 +5386,219 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5405,7 +5618,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5466,7 +5679,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5511,7 +5724,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8189,7 +8402,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:215 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>